<commit_message>
updated and cleaned up code
</commit_message>
<xml_diff>
--- a/Assignment_2_checklist.xlsx
+++ b/Assignment_2_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\AdvancedGamesProgrammingCGP600\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{589225AD-EC12-4E7C-B638-73D3153420FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CA4E1F28-4514-42AD-BECF-3578014A35A3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="2595" xr2:uid="{55536DC3-F3A6-4901-8C52-0177ACD9FD83}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="125">
   <si>
     <t>Report</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>% out of unit</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -803,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5441D33C-E496-40B9-9987-72D769C4F1A0}">
-  <dimension ref="A1:B131"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +865,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -892,7 +895,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -918,10 +921,10 @@
       <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1050,10 +1053,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="63.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="6"/>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1234,10 +1237,10 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="6"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -1644,7 +1647,7 @@
         <v>109</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -1728,7 +1731,7 @@
         <v>120</v>
       </c>
       <c r="B124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -1766,18 +1769,39 @@
       </c>
       <c r="B131">
         <f>SUM(B3:B5,B7:B9,B11:B13,B16:B18,B20:B22,B24:B25,B27:B28,B30,B32,B34:B36,B38:B39,B42:B44,B46:B48,B50:B52,B55:B57,B59:B61,B63:B65,B68:B70,B72:B74,B76:B78,B81:B82,B84:B85,B87:B89,B91:B93,B95:B97,B99:B100,B103:B105,B107:B109,B111:B116,B118:B121,B123:B125,B127:B129)</f>
-        <v>52</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B134">
+        <f>(B131/100)*75</f>
+        <v>42.000000000000007</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A49:B49"/>
     <mergeCell ref="A98:B98"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A66:B66"/>
@@ -1791,25 +1815,13 @@
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="A90:B90"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A122:B122"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>